<commit_message>
added omp_resolution data set
</commit_message>
<xml_diff>
--- a/smallpt/binary/omp_resolution.xlsx
+++ b/smallpt/binary/omp_resolution.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="omp_resolution" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -51,7 +51,7 @@
     <t>omp_samps</t>
   </si>
   <si>
-    <t>thread_pool</t>
+    <t>manual_mt</t>
   </si>
 </sst>
 </file>
@@ -861,7 +861,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,11 +917,12 @@
         <v>14.7788</v>
       </c>
       <c r="E3">
-        <v>0.156954121</v>
+        <f>D2/D3</f>
+        <v>6.3712886025929025</v>
       </c>
       <c r="F3">
         <f>E3/8</f>
-        <v>1.9619265125E-2</v>
+        <v>0.79641107532411282</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,11 +1038,12 @@
         <v>14.942600000000001</v>
       </c>
       <c r="E13">
-        <v>0.15869371299999999</v>
+        <f>D2/D13</f>
+        <v>6.3014468700226196</v>
       </c>
       <c r="F13">
         <f>E13/8</f>
-        <v>1.9836714124999998E-2</v>
+        <v>0.78768085875282745</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1157,11 +1159,12 @@
         <v>31.966699999999999</v>
       </c>
       <c r="E23">
-        <v>0.33949341500000002</v>
+        <f>D2/D23</f>
+        <v>2.9455652288162368</v>
       </c>
       <c r="F23">
         <f>E23/8</f>
-        <v>4.2436676875000003E-2</v>
+        <v>0.3681956536020296</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1277,12 +1280,12 @@
         <v>15.112399999999999</v>
       </c>
       <c r="E33">
-        <f>D33/D2</f>
-        <v>0.16049702633814783</v>
+        <f>D2/D33</f>
+        <v>6.2306450332177548</v>
       </c>
       <c r="F33">
         <f>E33/8</f>
-        <v>2.0062128292268479E-2</v>
+        <v>0.77883062915221934</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>